<commit_message>
update ui - bug fixed
</commit_message>
<xml_diff>
--- a/DATA/1.xlsx
+++ b/DATA/1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19872" windowHeight="7716"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$Q$500</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -6423,8 +6423,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6547,7 +6547,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -6582,7 +6581,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6758,16 +6756,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
-      <selection activeCell="J504" sqref="J504"/>
+      <selection activeCell="A489" sqref="A489:XFD489"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1">
         <v>4601</v>
       </c>
@@ -6809,7 +6807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>4601</v>
       </c>
@@ -6856,7 +6854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>4622</v>
       </c>
@@ -6892,7 +6890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>4627</v>
       </c>
@@ -6939,7 +6937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>4601</v>
       </c>
@@ -6981,7 +6979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>4601</v>
       </c>
@@ -7023,7 +7021,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>4601</v>
       </c>
@@ -7070,7 +7068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>4627</v>
       </c>
@@ -7117,7 +7115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>4601</v>
       </c>
@@ -7159,7 +7157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>4621</v>
       </c>
@@ -7201,7 +7199,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>4615</v>
       </c>
@@ -7242,7 +7240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>4618</v>
       </c>
@@ -7289,7 +7287,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>4604</v>
       </c>
@@ -7336,7 +7334,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>4601</v>
       </c>
@@ -7392,7 +7390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>4612</v>
       </c>
@@ -7434,7 +7432,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>4612</v>
       </c>
@@ -7476,7 +7474,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>4614</v>
       </c>
@@ -7514,7 +7512,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>4624</v>
       </c>
@@ -7561,7 +7559,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>4626</v>
       </c>
@@ -7603,7 +7601,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>4601</v>
       </c>
@@ -7645,7 +7643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>4601</v>
       </c>
@@ -7692,7 +7690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>4619</v>
       </c>
@@ -7733,7 +7731,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>4619</v>
       </c>
@@ -7780,7 +7778,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>4612</v>
       </c>
@@ -7821,7 +7819,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>4601</v>
       </c>
@@ -7863,7 +7861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>4616</v>
       </c>
@@ -7910,7 +7908,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>4612</v>
       </c>
@@ -7957,7 +7955,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>4602</v>
       </c>
@@ -8004,7 +8002,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>4614</v>
       </c>
@@ -8051,7 +8049,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26">
       <c r="A30">
         <v>4602</v>
       </c>
@@ -8098,7 +8096,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26">
       <c r="A31">
         <v>4627</v>
       </c>
@@ -8145,7 +8143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26">
       <c r="A32">
         <v>4616</v>
       </c>
@@ -8181,7 +8179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26">
       <c r="A33">
         <v>4601</v>
       </c>
@@ -8231,7 +8229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26">
       <c r="A34">
         <v>4601</v>
       </c>
@@ -8278,7 +8276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26">
       <c r="A35">
         <v>4601</v>
       </c>
@@ -8320,7 +8318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26">
       <c r="A36">
         <v>4607</v>
       </c>
@@ -8367,7 +8365,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26">
       <c r="A37">
         <v>4601</v>
       </c>
@@ -8414,7 +8412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26">
       <c r="A38">
         <v>4627</v>
       </c>
@@ -8456,7 +8454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26">
       <c r="A39">
         <v>4625</v>
       </c>
@@ -8503,7 +8501,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26">
       <c r="A40">
         <v>4601</v>
       </c>
@@ -8550,7 +8548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26">
       <c r="A41">
         <v>4612</v>
       </c>
@@ -8597,7 +8595,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26">
       <c r="A42">
         <v>4624</v>
       </c>
@@ -8639,7 +8637,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26">
       <c r="A43">
         <v>4616</v>
       </c>
@@ -8686,7 +8684,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26">
       <c r="A44">
         <v>4625</v>
       </c>
@@ -8733,7 +8731,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26">
       <c r="A45">
         <v>4627</v>
       </c>
@@ -8780,7 +8778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26">
       <c r="A46">
         <v>4616</v>
       </c>
@@ -8821,7 +8819,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26">
       <c r="A47">
         <v>4601</v>
       </c>
@@ -8868,7 +8866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26">
       <c r="A48">
         <v>4616</v>
       </c>
@@ -8910,7 +8908,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26">
       <c r="A49">
         <v>4601</v>
       </c>
@@ -8957,7 +8955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26">
       <c r="A50">
         <v>4607</v>
       </c>
@@ -8993,7 +8991,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26">
       <c r="A51">
         <v>4612</v>
       </c>
@@ -9040,7 +9038,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26">
       <c r="A52">
         <v>4603</v>
       </c>
@@ -9087,7 +9085,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26">
       <c r="A53">
         <v>4601</v>
       </c>
@@ -9134,7 +9132,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26">
       <c r="A54">
         <v>4601</v>
       </c>
@@ -9184,7 +9182,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26">
       <c r="A55">
         <v>4620</v>
       </c>
@@ -9231,7 +9229,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26">
       <c r="A56">
         <v>4628</v>
       </c>
@@ -9272,7 +9270,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26">
       <c r="A57">
         <v>4608</v>
       </c>
@@ -9319,7 +9317,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26">
       <c r="A58">
         <v>4601</v>
       </c>
@@ -9366,7 +9364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26">
       <c r="A59">
         <v>4612</v>
       </c>
@@ -9419,7 +9417,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26">
       <c r="A60">
         <v>4604</v>
       </c>
@@ -9466,7 +9464,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26">
       <c r="A61">
         <v>4627</v>
       </c>
@@ -9513,7 +9511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26">
       <c r="A62">
         <v>4601</v>
       </c>
@@ -9555,7 +9553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26">
       <c r="A63">
         <v>4619</v>
       </c>
@@ -9597,7 +9595,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26">
       <c r="A64">
         <v>4627</v>
       </c>
@@ -9644,7 +9642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26">
       <c r="A65">
         <v>4601</v>
       </c>
@@ -9691,7 +9689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26">
       <c r="A66">
         <v>4624</v>
       </c>
@@ -9738,7 +9736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26">
       <c r="A67">
         <v>4624</v>
       </c>
@@ -9785,7 +9783,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26">
       <c r="A68">
         <v>4616</v>
       </c>
@@ -9826,7 +9824,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26">
       <c r="A69">
         <v>4621</v>
       </c>
@@ -9873,7 +9871,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26">
       <c r="A70">
         <v>4602</v>
       </c>
@@ -9915,7 +9913,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26">
       <c r="A71">
         <v>4603</v>
       </c>
@@ -9957,7 +9955,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26">
       <c r="A72">
         <v>4619</v>
       </c>
@@ -9993,7 +9991,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26">
       <c r="A73">
         <v>4605</v>
       </c>
@@ -10043,7 +10041,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26">
       <c r="A74">
         <v>4628</v>
       </c>
@@ -10090,7 +10088,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26">
       <c r="A75">
         <v>4610</v>
       </c>
@@ -10132,7 +10130,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26">
       <c r="A76">
         <v>4612</v>
       </c>
@@ -10174,7 +10172,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26">
       <c r="A77">
         <v>4601</v>
       </c>
@@ -10215,7 +10213,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26">
       <c r="A78">
         <v>4605</v>
       </c>
@@ -10256,7 +10254,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26">
       <c r="A79">
         <v>4602</v>
       </c>
@@ -10297,7 +10295,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26">
       <c r="A80">
         <v>4601</v>
       </c>
@@ -10339,7 +10337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26">
       <c r="A81">
         <v>4602</v>
       </c>
@@ -10380,7 +10378,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26">
       <c r="A82">
         <v>4627</v>
       </c>
@@ -10424,7 +10422,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26">
       <c r="A83">
         <v>4602</v>
       </c>
@@ -10465,7 +10463,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26">
       <c r="A84">
         <v>4621</v>
       </c>
@@ -10512,7 +10510,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26">
       <c r="A85">
         <v>4627</v>
       </c>
@@ -10562,7 +10560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26">
       <c r="A86">
         <v>4601</v>
       </c>
@@ -10609,7 +10607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26">
       <c r="A87">
         <v>4612</v>
       </c>
@@ -10657,7 +10655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26">
       <c r="A88">
         <v>4619</v>
       </c>
@@ -10696,7 +10694,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26">
       <c r="A89">
         <v>4618</v>
       </c>
@@ -10738,7 +10736,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26">
       <c r="A90">
         <v>4615</v>
       </c>
@@ -10791,7 +10789,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26">
       <c r="A91">
         <v>4621</v>
       </c>
@@ -10827,7 +10825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26">
       <c r="A92">
         <v>4601</v>
       </c>
@@ -10863,7 +10861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26">
       <c r="A93">
         <v>4601</v>
       </c>
@@ -10905,7 +10903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26">
       <c r="A94">
         <v>4603</v>
       </c>
@@ -10947,7 +10945,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26">
       <c r="A95">
         <v>4601</v>
       </c>
@@ -10988,7 +10986,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26">
       <c r="A96">
         <v>4621</v>
       </c>
@@ -11030,7 +11028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26">
       <c r="A97">
         <v>4627</v>
       </c>
@@ -11077,7 +11075,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26">
       <c r="A98">
         <v>4601</v>
       </c>
@@ -11124,7 +11122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26">
       <c r="A99">
         <v>4612</v>
       </c>
@@ -11166,7 +11164,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26">
       <c r="A100">
         <v>4603</v>
       </c>
@@ -11207,7 +11205,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26">
       <c r="A101">
         <v>4602</v>
       </c>
@@ -11243,7 +11241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26">
       <c r="A102">
         <v>4612</v>
       </c>
@@ -11287,7 +11285,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26">
       <c r="A103">
         <v>4607</v>
       </c>
@@ -11334,7 +11332,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26">
       <c r="A104">
         <v>4601</v>
       </c>
@@ -11375,7 +11373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26">
       <c r="A105">
         <v>4603</v>
       </c>
@@ -11416,7 +11414,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26">
       <c r="A106">
         <v>4610</v>
       </c>
@@ -11463,7 +11461,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26">
       <c r="A107">
         <v>4601</v>
       </c>
@@ -11505,7 +11503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26">
       <c r="A108">
         <v>4601</v>
       </c>
@@ -11546,7 +11544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26">
       <c r="A109">
         <v>4601</v>
       </c>
@@ -11587,7 +11585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26">
       <c r="A110">
         <v>4604</v>
       </c>
@@ -11629,7 +11627,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26">
       <c r="A111">
         <v>4608</v>
       </c>
@@ -11670,7 +11668,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26">
       <c r="A112">
         <v>4616</v>
       </c>
@@ -11717,7 +11715,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26">
       <c r="A113">
         <v>4612</v>
       </c>
@@ -11758,7 +11756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26">
       <c r="A114">
         <v>4610</v>
       </c>
@@ -11799,7 +11797,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26">
       <c r="A115">
         <v>4627</v>
       </c>
@@ -11840,7 +11838,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26">
       <c r="A116">
         <v>4608</v>
       </c>
@@ -11890,7 +11888,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26">
       <c r="A117">
         <v>4627</v>
       </c>
@@ -11931,7 +11929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26">
       <c r="A118">
         <v>4618</v>
       </c>
@@ -11975,7 +11973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26">
       <c r="A119">
         <v>4612</v>
       </c>
@@ -12016,7 +12014,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26">
       <c r="A120">
         <v>4616</v>
       </c>
@@ -12064,7 +12062,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:26">
       <c r="A121">
         <v>4622</v>
       </c>
@@ -12111,7 +12109,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26">
       <c r="A122">
         <v>4607</v>
       </c>
@@ -12152,7 +12150,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26">
       <c r="A123">
         <v>4601</v>
       </c>
@@ -12199,7 +12197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26">
       <c r="A124">
         <v>4625</v>
       </c>
@@ -12241,7 +12239,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26">
       <c r="A125">
         <v>4624</v>
       </c>
@@ -12283,7 +12281,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26">
       <c r="A126">
         <v>4605</v>
       </c>
@@ -12324,7 +12322,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26">
       <c r="A127">
         <v>4621</v>
       </c>
@@ -12366,7 +12364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26">
       <c r="A128">
         <v>4601</v>
       </c>
@@ -12413,7 +12411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26">
       <c r="A129">
         <v>4624</v>
       </c>
@@ -12454,7 +12452,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:26">
       <c r="A130">
         <v>4603</v>
       </c>
@@ -12490,7 +12488,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26">
       <c r="A131">
         <v>4627</v>
       </c>
@@ -12531,7 +12529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:26">
       <c r="A132">
         <v>4612</v>
       </c>
@@ -12567,7 +12565,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:26">
       <c r="A133">
         <v>4627</v>
       </c>
@@ -12609,7 +12607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:26">
       <c r="A134">
         <v>4601</v>
       </c>
@@ -12656,7 +12654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:26">
       <c r="A135">
         <v>4602</v>
       </c>
@@ -12697,7 +12695,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:26">
       <c r="A136">
         <v>4608</v>
       </c>
@@ -12744,7 +12742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:26">
       <c r="A137">
         <v>4628</v>
       </c>
@@ -12785,7 +12783,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:26">
       <c r="A138">
         <v>4618</v>
       </c>
@@ -12829,7 +12827,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:26">
       <c r="A139">
         <v>4618</v>
       </c>
@@ -12871,7 +12869,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:26">
       <c r="A140">
         <v>4624</v>
       </c>
@@ -12918,7 +12916,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:26">
       <c r="A141">
         <v>4604</v>
       </c>
@@ -12959,7 +12957,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:26">
       <c r="A142">
         <v>4601</v>
       </c>
@@ -13001,7 +12999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:26">
       <c r="A143">
         <v>4611</v>
       </c>
@@ -13048,7 +13046,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:26">
       <c r="A144">
         <v>4612</v>
       </c>
@@ -13095,7 +13093,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26">
       <c r="A145">
         <v>4619</v>
       </c>
@@ -13136,7 +13134,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26">
       <c r="A146">
         <v>4605</v>
       </c>
@@ -13177,7 +13175,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:26">
       <c r="A147">
         <v>4607</v>
       </c>
@@ -13221,7 +13219,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:26">
       <c r="A148">
         <v>4601</v>
       </c>
@@ -13268,7 +13266,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26">
       <c r="A149">
         <v>4604</v>
       </c>
@@ -13321,7 +13319,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:26">
       <c r="A150">
         <v>4602</v>
       </c>
@@ -13368,7 +13366,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:26">
       <c r="A151">
         <v>4627</v>
       </c>
@@ -13409,7 +13407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26">
       <c r="A152">
         <v>4616</v>
       </c>
@@ -13453,7 +13451,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:26">
       <c r="A153">
         <v>4619</v>
       </c>
@@ -13489,7 +13487,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26">
       <c r="A154">
         <v>4614</v>
       </c>
@@ -13530,7 +13528,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26">
       <c r="A155">
         <v>4627</v>
       </c>
@@ -13577,7 +13575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:26">
       <c r="A156">
         <v>4627</v>
       </c>
@@ -13618,7 +13616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:26">
       <c r="A157">
         <v>4601</v>
       </c>
@@ -13660,7 +13658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:26">
       <c r="A158">
         <v>4626</v>
       </c>
@@ -13707,7 +13705,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:26">
       <c r="A159">
         <v>4601</v>
       </c>
@@ -13743,7 +13741,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:26">
       <c r="A160">
         <v>4616</v>
       </c>
@@ -13779,7 +13777,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26">
       <c r="A161">
         <v>4601</v>
       </c>
@@ -13826,7 +13824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26">
       <c r="A162">
         <v>4612</v>
       </c>
@@ -13867,7 +13865,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26">
       <c r="A163">
         <v>4621</v>
       </c>
@@ -13909,7 +13907,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:26">
       <c r="A164">
         <v>4621</v>
       </c>
@@ -13945,7 +13943,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:26">
       <c r="A165">
         <v>4601</v>
       </c>
@@ -13995,7 +13993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:26">
       <c r="A166">
         <v>4601</v>
       </c>
@@ -14031,7 +14029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:26">
       <c r="A167">
         <v>4601</v>
       </c>
@@ -14078,7 +14076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:26">
       <c r="A168">
         <v>4601</v>
       </c>
@@ -14119,7 +14117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:26">
       <c r="A169">
         <v>4603</v>
       </c>
@@ -14160,7 +14158,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:26">
       <c r="A170">
         <v>4601</v>
       </c>
@@ -14202,7 +14200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:26">
       <c r="A171">
         <v>4604</v>
       </c>
@@ -14246,7 +14244,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:26">
       <c r="A172">
         <v>4601</v>
       </c>
@@ -14287,7 +14285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:26">
       <c r="A173">
         <v>4603</v>
       </c>
@@ -14323,7 +14321,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:26">
       <c r="A174">
         <v>4601</v>
       </c>
@@ -14373,7 +14371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:26">
       <c r="A175">
         <v>4601</v>
       </c>
@@ -14420,7 +14418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:26">
       <c r="A176">
         <v>4601</v>
       </c>
@@ -14462,7 +14460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:26">
       <c r="A177">
         <v>4619</v>
       </c>
@@ -14504,7 +14502,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26">
       <c r="A178">
         <v>4618</v>
       </c>
@@ -14551,7 +14549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26">
       <c r="A179">
         <v>4602</v>
       </c>
@@ -14593,7 +14591,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26">
       <c r="A180">
         <v>4620</v>
       </c>
@@ -14635,7 +14633,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:26">
       <c r="A181">
         <v>4620</v>
       </c>
@@ -14677,7 +14675,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="182" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:26">
       <c r="A182">
         <v>4627</v>
       </c>
@@ -14724,7 +14722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:26">
       <c r="A183">
         <v>4624</v>
       </c>
@@ -14771,7 +14769,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="184" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:26">
       <c r="A184">
         <v>4612</v>
       </c>
@@ -14807,7 +14805,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="185" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:26">
       <c r="A185">
         <v>4601</v>
       </c>
@@ -14854,7 +14852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:26">
       <c r="A186">
         <v>4618</v>
       </c>
@@ -14896,7 +14894,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="187" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:26">
       <c r="A187">
         <v>4603</v>
       </c>
@@ -14938,7 +14936,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="188" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:26">
       <c r="A188">
         <v>4601</v>
       </c>
@@ -14979,7 +14977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:26">
       <c r="A189">
         <v>4602</v>
       </c>
@@ -15020,7 +15018,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:26">
       <c r="A190">
         <v>4616</v>
       </c>
@@ -15062,7 +15060,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:26">
       <c r="A191">
         <v>4612</v>
       </c>
@@ -15103,7 +15101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="192" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:26">
       <c r="A192">
         <v>4601</v>
       </c>
@@ -15150,7 +15148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:26">
       <c r="A193">
         <v>4611</v>
       </c>
@@ -15186,7 +15184,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:26">
       <c r="A194">
         <v>4602</v>
       </c>
@@ -15233,7 +15231,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:26">
       <c r="A195">
         <v>4601</v>
       </c>
@@ -15280,7 +15278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:26">
       <c r="A196">
         <v>4627</v>
       </c>
@@ -15327,7 +15325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:26">
       <c r="A197">
         <v>4601</v>
       </c>
@@ -15368,7 +15366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:26">
       <c r="A198">
         <v>4612</v>
       </c>
@@ -15409,7 +15407,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:26">
       <c r="A199">
         <v>4624</v>
       </c>
@@ -15451,7 +15449,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:26">
       <c r="A200">
         <v>4607</v>
       </c>
@@ -15498,7 +15496,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:26">
       <c r="A201">
         <v>4620</v>
       </c>
@@ -15551,7 +15549,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:26">
       <c r="A202">
         <v>4628</v>
       </c>
@@ -15592,7 +15590,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="203" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:26">
       <c r="A203">
         <v>4627</v>
       </c>
@@ -15639,7 +15637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:26">
       <c r="A204">
         <v>4601</v>
       </c>
@@ -15686,7 +15684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:26">
       <c r="A205">
         <v>4601</v>
       </c>
@@ -15727,7 +15725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:26">
       <c r="A206">
         <v>4613</v>
       </c>
@@ -15774,7 +15772,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="207" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:26">
       <c r="A207">
         <v>4605</v>
       </c>
@@ -15815,7 +15813,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="208" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:26">
       <c r="A208">
         <v>4624</v>
       </c>
@@ -15862,7 +15860,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:26">
       <c r="A209">
         <v>4601</v>
       </c>
@@ -15898,7 +15896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:26">
       <c r="A210">
         <v>4601</v>
       </c>
@@ -15939,7 +15937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:26">
       <c r="A211">
         <v>4601</v>
       </c>
@@ -15986,7 +15984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:26">
       <c r="A212">
         <v>4602</v>
       </c>
@@ -16027,7 +16025,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:26">
       <c r="A213">
         <v>4618</v>
       </c>
@@ -16068,7 +16066,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:26">
       <c r="A214">
         <v>4627</v>
       </c>
@@ -16104,7 +16102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:26">
       <c r="A215">
         <v>4627</v>
       </c>
@@ -16151,7 +16149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:26">
       <c r="A216">
         <v>4625</v>
       </c>
@@ -16193,7 +16191,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:26">
       <c r="A217">
         <v>4625</v>
       </c>
@@ -16240,7 +16238,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:26">
       <c r="A218">
         <v>4601</v>
       </c>
@@ -16287,7 +16285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:26">
       <c r="A219">
         <v>4607</v>
       </c>
@@ -16334,7 +16332,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:26">
       <c r="A220">
         <v>4601</v>
       </c>
@@ -16375,7 +16373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:26">
       <c r="A221">
         <v>4619</v>
       </c>
@@ -16414,7 +16412,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:26">
       <c r="A222">
         <v>4602</v>
       </c>
@@ -16450,7 +16448,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="223" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:26">
       <c r="A223">
         <v>4601</v>
       </c>
@@ -16497,7 +16495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:26">
       <c r="A224">
         <v>4624</v>
       </c>
@@ -16550,7 +16548,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="225" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:26">
       <c r="A225">
         <v>4601</v>
       </c>
@@ -16591,7 +16589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:26">
       <c r="A226">
         <v>4609</v>
       </c>
@@ -16627,7 +16625,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="227" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:26">
       <c r="A227">
         <v>4605</v>
       </c>
@@ -16668,7 +16666,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="228" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:26">
       <c r="A228">
         <v>4627</v>
       </c>
@@ -16715,7 +16713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:26">
       <c r="A229">
         <v>4627</v>
       </c>
@@ -16762,7 +16760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:26">
       <c r="A230">
         <v>4603</v>
       </c>
@@ -16803,7 +16801,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="231" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:26">
       <c r="A231">
         <v>4601</v>
       </c>
@@ -16845,7 +16843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:26">
       <c r="A232">
         <v>4621</v>
       </c>
@@ -16892,7 +16890,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="233" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:26">
       <c r="A233">
         <v>4612</v>
       </c>
@@ -16939,7 +16937,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="234" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:26">
       <c r="A234">
         <v>4602</v>
       </c>
@@ -16980,7 +16978,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="235" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:26">
       <c r="A235">
         <v>4616</v>
       </c>
@@ -17021,7 +17019,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="236" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:26">
       <c r="A236">
         <v>4601</v>
       </c>
@@ -17063,7 +17061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:26">
       <c r="A237">
         <v>4611</v>
       </c>
@@ -17110,7 +17108,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="238" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:26">
       <c r="A238">
         <v>4603</v>
       </c>
@@ -17151,7 +17149,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="239" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:26">
       <c r="A239">
         <v>4626</v>
       </c>
@@ -17189,7 +17187,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="240" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:26">
       <c r="A240">
         <v>4605</v>
       </c>
@@ -17236,7 +17234,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="241" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:26">
       <c r="A241">
         <v>4624</v>
       </c>
@@ -17283,7 +17281,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:26">
       <c r="A242">
         <v>4601</v>
       </c>
@@ -17330,7 +17328,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:26">
       <c r="A243">
         <v>4618</v>
       </c>
@@ -17380,7 +17378,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:26">
       <c r="A244">
         <v>4601</v>
       </c>
@@ -17416,7 +17414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:26">
       <c r="A245">
         <v>4601</v>
       </c>
@@ -17463,7 +17461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:26">
       <c r="A246">
         <v>4609</v>
       </c>
@@ -17510,7 +17508,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:26">
       <c r="A247">
         <v>4612</v>
       </c>
@@ -17557,7 +17555,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:26">
       <c r="A248">
         <v>4627</v>
       </c>
@@ -17604,7 +17602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:26">
       <c r="A249">
         <v>4601</v>
       </c>
@@ -17651,7 +17649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:26">
       <c r="A250">
         <v>4627</v>
       </c>
@@ -17698,7 +17696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:26">
       <c r="A251">
         <v>4612</v>
       </c>
@@ -17740,7 +17738,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:26">
       <c r="A252">
         <v>4616</v>
       </c>
@@ -17787,7 +17785,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:26">
       <c r="A253">
         <v>4616</v>
       </c>
@@ -17828,7 +17826,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:26">
       <c r="A254">
         <v>4621</v>
       </c>
@@ -17875,7 +17873,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:26">
       <c r="A255">
         <v>4606</v>
       </c>
@@ -17916,7 +17914,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:26">
       <c r="A256">
         <v>4610</v>
       </c>
@@ -17963,7 +17961,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="257" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:26">
       <c r="A257">
         <v>4611</v>
       </c>
@@ -17999,7 +17997,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="258" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:26">
       <c r="A258">
         <v>4602</v>
       </c>
@@ -18040,7 +18038,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="259" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:26">
       <c r="A259">
         <v>4604</v>
       </c>
@@ -18076,7 +18074,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="260" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:26">
       <c r="A260">
         <v>4606</v>
       </c>
@@ -18112,7 +18110,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="261" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:26">
       <c r="A261">
         <v>4615</v>
       </c>
@@ -18153,7 +18151,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="262" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:26">
       <c r="A262">
         <v>4615</v>
       </c>
@@ -18195,7 +18193,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="263" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:26">
       <c r="A263">
         <v>4612</v>
       </c>
@@ -18236,7 +18234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="264" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:26">
       <c r="A264">
         <v>4602</v>
       </c>
@@ -18277,7 +18275,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="265" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:26">
       <c r="A265">
         <v>4601</v>
       </c>
@@ -18324,7 +18322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:26">
       <c r="A266">
         <v>4604</v>
       </c>
@@ -18366,7 +18364,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="267" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:26">
       <c r="A267">
         <v>4607</v>
       </c>
@@ -18413,7 +18411,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="268" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:26">
       <c r="A268">
         <v>4601</v>
       </c>
@@ -18454,7 +18452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:26">
       <c r="A269">
         <v>4627</v>
       </c>
@@ -18501,7 +18499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="270" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:26">
       <c r="A270">
         <v>4607</v>
       </c>
@@ -18537,7 +18535,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="271" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:26">
       <c r="A271">
         <v>4612</v>
       </c>
@@ -18573,7 +18571,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="272" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:26">
       <c r="A272">
         <v>4601</v>
       </c>
@@ -18614,7 +18612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:26">
       <c r="A273">
         <v>4602</v>
       </c>
@@ -18650,7 +18648,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="274" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:26">
       <c r="A274">
         <v>4602</v>
       </c>
@@ -18691,7 +18689,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="275" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:26">
       <c r="A275">
         <v>4601</v>
       </c>
@@ -18738,7 +18736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:26">
       <c r="A276">
         <v>4612</v>
       </c>
@@ -18779,7 +18777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="277" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:26">
       <c r="A277">
         <v>4614</v>
       </c>
@@ -18826,7 +18824,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="278" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:26">
       <c r="A278">
         <v>4601</v>
       </c>
@@ -18870,7 +18868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="279" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:26">
       <c r="A279">
         <v>4621</v>
       </c>
@@ -18917,7 +18915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="280" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:26">
       <c r="A280">
         <v>4601</v>
       </c>
@@ -18953,7 +18951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:26">
       <c r="A281">
         <v>4601</v>
       </c>
@@ -18989,7 +18987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:26">
       <c r="A282">
         <v>4616</v>
       </c>
@@ -19025,7 +19023,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="283" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:26">
       <c r="A283">
         <v>4618</v>
       </c>
@@ -19067,7 +19065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="284" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:26">
       <c r="A284">
         <v>4621</v>
       </c>
@@ -19103,7 +19101,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="285" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:26">
       <c r="A285">
         <v>4612</v>
       </c>
@@ -19156,7 +19154,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="286" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:26">
       <c r="A286">
         <v>4605</v>
       </c>
@@ -19192,7 +19190,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="287" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:26">
       <c r="A287">
         <v>4604</v>
       </c>
@@ -19233,7 +19231,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="288" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:26">
       <c r="A288">
         <v>4624</v>
       </c>
@@ -19275,7 +19273,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="289" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:26">
       <c r="A289">
         <v>4608</v>
       </c>
@@ -19322,7 +19320,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="290" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:26">
       <c r="A290">
         <v>4624</v>
       </c>
@@ -19375,7 +19373,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="291" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:26">
       <c r="A291">
         <v>4627</v>
       </c>
@@ -19422,7 +19420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="292" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:26">
       <c r="A292">
         <v>4606</v>
       </c>
@@ -19469,7 +19467,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="293" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:26">
       <c r="A293">
         <v>4604</v>
       </c>
@@ -19516,7 +19514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="294" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:26">
       <c r="A294">
         <v>4612</v>
       </c>
@@ -19558,7 +19556,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="295" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:26">
       <c r="A295">
         <v>4612</v>
       </c>
@@ -19594,7 +19592,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="296" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:26">
       <c r="A296">
         <v>4601</v>
       </c>
@@ -19641,7 +19639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="297" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:26">
       <c r="A297">
         <v>4601</v>
       </c>
@@ -19677,7 +19675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="298" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:26">
       <c r="A298">
         <v>4627</v>
       </c>
@@ -19718,7 +19716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:26">
       <c r="A299">
         <v>4621</v>
       </c>
@@ -19759,7 +19757,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="300" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:26">
       <c r="A300">
         <v>4618</v>
       </c>
@@ -19800,7 +19798,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="301" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:26">
       <c r="A301">
         <v>4627</v>
       </c>
@@ -19841,7 +19839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="302" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:26">
       <c r="A302">
         <v>4607</v>
       </c>
@@ -19883,7 +19881,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="303" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:26">
       <c r="A303">
         <v>4602</v>
       </c>
@@ -19927,7 +19925,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="304" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:26">
       <c r="A304">
         <v>4601</v>
       </c>
@@ -19974,7 +19972,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="305" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:26">
       <c r="A305">
         <v>4612</v>
       </c>
@@ -20021,7 +20019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="306" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:26">
       <c r="A306">
         <v>4602</v>
       </c>
@@ -20068,7 +20066,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="307" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:26">
       <c r="A307">
         <v>4601</v>
       </c>
@@ -20115,7 +20113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:26">
       <c r="A308">
         <v>4608</v>
       </c>
@@ -20156,7 +20154,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="309" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:26">
       <c r="A309">
         <v>4601</v>
       </c>
@@ -20197,7 +20195,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="310" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:26">
       <c r="A310">
         <v>4601</v>
       </c>
@@ -20238,7 +20236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="311" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:26">
       <c r="A311">
         <v>4601</v>
       </c>
@@ -20280,7 +20278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="312" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:26">
       <c r="A312">
         <v>4602</v>
       </c>
@@ -20321,7 +20319,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="313" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:26">
       <c r="A313">
         <v>4605</v>
       </c>
@@ -20362,7 +20360,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="314" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:26">
       <c r="A314">
         <v>4601</v>
       </c>
@@ -20404,7 +20402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="315" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:26">
       <c r="A315">
         <v>4623</v>
       </c>
@@ -20446,7 +20444,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="316" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:26">
       <c r="A316">
         <v>4619</v>
       </c>
@@ -20487,7 +20485,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="317" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:26">
       <c r="A317">
         <v>4608</v>
       </c>
@@ -20534,7 +20532,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="318" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:26">
       <c r="A318">
         <v>4612</v>
       </c>
@@ -20570,7 +20568,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="319" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:26">
       <c r="A319">
         <v>4603</v>
       </c>
@@ -20617,7 +20615,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="320" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:26">
       <c r="A320">
         <v>4616</v>
       </c>
@@ -20658,7 +20656,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="321" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:26">
       <c r="A321">
         <v>4601</v>
       </c>
@@ -20699,7 +20697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="322" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:26">
       <c r="A322">
         <v>4601</v>
       </c>
@@ -20740,7 +20738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="323" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:26">
       <c r="A323">
         <v>4605</v>
       </c>
@@ -20790,7 +20788,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="324" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:26">
       <c r="A324">
         <v>4626</v>
       </c>
@@ -20832,7 +20830,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="325" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:26">
       <c r="A325">
         <v>4601</v>
       </c>
@@ -20879,7 +20877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="326" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:26">
       <c r="A326">
         <v>4618</v>
       </c>
@@ -20920,7 +20918,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="327" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:26">
       <c r="A327">
         <v>4601</v>
       </c>
@@ -20967,7 +20965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="328" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:26">
       <c r="A328">
         <v>4624</v>
       </c>
@@ -21008,7 +21006,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="329" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:26">
       <c r="A329">
         <v>4609</v>
       </c>
@@ -21055,7 +21053,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="330" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:26">
       <c r="A330">
         <v>4612</v>
       </c>
@@ -21091,7 +21089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="331" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:26">
       <c r="A331">
         <v>4601</v>
       </c>
@@ -21138,7 +21136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="332" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:26">
       <c r="A332">
         <v>4609</v>
       </c>
@@ -21179,7 +21177,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="333" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:26">
       <c r="A333">
         <v>4601</v>
       </c>
@@ -21220,7 +21218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="334" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:26">
       <c r="A334">
         <v>4610</v>
       </c>
@@ -21267,7 +21265,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:26">
       <c r="A335">
         <v>4614</v>
       </c>
@@ -21311,7 +21309,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="336" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:26">
       <c r="A336">
         <v>4612</v>
       </c>
@@ -21353,7 +21351,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="337" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:26">
       <c r="A337">
         <v>4612</v>
       </c>
@@ -21397,7 +21395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="338" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:26">
       <c r="A338">
         <v>4601</v>
       </c>
@@ -21438,7 +21436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="339" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:26">
       <c r="A339">
         <v>4608</v>
       </c>
@@ -21485,7 +21483,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="340" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:26">
       <c r="A340">
         <v>4609</v>
       </c>
@@ -21526,7 +21524,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="341" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:26">
       <c r="A341">
         <v>4621</v>
       </c>
@@ -21573,7 +21571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="342" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:26">
       <c r="A342">
         <v>4601</v>
       </c>
@@ -21614,7 +21612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="343" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:26">
       <c r="A343">
         <v>4601</v>
       </c>
@@ -21655,7 +21653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="344" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:26">
       <c r="A344">
         <v>4601</v>
       </c>
@@ -21697,7 +21695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="345" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:26">
       <c r="A345">
         <v>4606</v>
       </c>
@@ -21733,7 +21731,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="346" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:26">
       <c r="A346">
         <v>4624</v>
       </c>
@@ -21774,7 +21772,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="347" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:26">
       <c r="A347">
         <v>4609</v>
       </c>
@@ -21815,7 +21813,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="348" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:26">
       <c r="A348">
         <v>4601</v>
       </c>
@@ -21859,7 +21857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="349" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:26">
       <c r="A349">
         <v>4609</v>
       </c>
@@ -21903,7 +21901,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="350" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:26">
       <c r="A350">
         <v>4624</v>
       </c>
@@ -21950,7 +21948,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="351" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:26">
       <c r="A351">
         <v>4602</v>
       </c>
@@ -21991,7 +21989,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="352" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:26">
       <c r="A352">
         <v>4607</v>
       </c>
@@ -22032,7 +22030,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="353" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:26">
       <c r="A353">
         <v>4607</v>
       </c>
@@ -22074,7 +22072,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="354" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:26">
       <c r="A354">
         <v>4624</v>
       </c>
@@ -22121,7 +22119,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="355" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:26">
       <c r="A355">
         <v>4602</v>
       </c>
@@ -22162,7 +22160,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="356" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:26">
       <c r="A356">
         <v>4624</v>
       </c>
@@ -22209,7 +22207,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="357" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:26">
       <c r="A357">
         <v>4601</v>
       </c>
@@ -22250,7 +22248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:26">
       <c r="A358">
         <v>4601</v>
       </c>
@@ -22291,7 +22289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:26">
       <c r="A359">
         <v>4625</v>
       </c>
@@ -22332,7 +22330,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="360" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:26">
       <c r="A360">
         <v>4601</v>
       </c>
@@ -22379,7 +22377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="361" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:26">
       <c r="A361">
         <v>4604</v>
       </c>
@@ -22426,7 +22424,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="362" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:26">
       <c r="A362">
         <v>4601</v>
       </c>
@@ -22467,7 +22465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="363" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:26">
       <c r="A363">
         <v>4601</v>
       </c>
@@ -22514,7 +22512,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="364" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:26">
       <c r="A364">
         <v>4602</v>
       </c>
@@ -22555,7 +22553,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="365" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:26">
       <c r="A365">
         <v>4601</v>
       </c>
@@ -22596,7 +22594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="366" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:26">
       <c r="A366">
         <v>4602</v>
       </c>
@@ -22637,7 +22635,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="367" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:26">
       <c r="A367">
         <v>4609</v>
       </c>
@@ -22679,7 +22677,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="368" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:26">
       <c r="A368">
         <v>4610</v>
       </c>
@@ -22718,7 +22716,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="369" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:26">
       <c r="A369">
         <v>4622</v>
       </c>
@@ -22754,7 +22752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="370" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:26">
       <c r="A370">
         <v>4624</v>
       </c>
@@ -22795,7 +22793,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="371" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:26">
       <c r="A371">
         <v>4624</v>
       </c>
@@ -22842,7 +22840,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="372" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:26">
       <c r="A372">
         <v>4625</v>
       </c>
@@ -22889,7 +22887,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="373" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:26">
       <c r="A373">
         <v>4628</v>
       </c>
@@ -22936,7 +22934,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="374" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:26">
       <c r="A374">
         <v>4601</v>
       </c>
@@ -22977,7 +22975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="375" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:26">
       <c r="A375">
         <v>4616</v>
       </c>
@@ -23024,7 +23022,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="376" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:26">
       <c r="A376">
         <v>4601</v>
       </c>
@@ -23071,7 +23069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="377" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:26">
       <c r="A377">
         <v>4601</v>
       </c>
@@ -23118,7 +23116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="378" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:26">
       <c r="A378">
         <v>4604</v>
       </c>
@@ -23159,7 +23157,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="379" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:26">
       <c r="A379">
         <v>4612</v>
       </c>
@@ -23206,7 +23204,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="380" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:26">
       <c r="A380">
         <v>4601</v>
       </c>
@@ -23253,7 +23251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="381" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:26">
       <c r="A381">
         <v>4621</v>
       </c>
@@ -23306,7 +23304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="382" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:26">
       <c r="A382">
         <v>4624</v>
       </c>
@@ -23353,7 +23351,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="383" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:26">
       <c r="A383">
         <v>4613</v>
       </c>
@@ -23389,7 +23387,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="384" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:26">
       <c r="A384">
         <v>4627</v>
       </c>
@@ -23436,7 +23434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="385" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:26">
       <c r="A385">
         <v>4601</v>
       </c>
@@ -23477,7 +23475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="386" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:26">
       <c r="A386">
         <v>4624</v>
       </c>
@@ -23518,7 +23516,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="387" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:26">
       <c r="A387">
         <v>4616</v>
       </c>
@@ -23565,7 +23563,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="388" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:26">
       <c r="A388">
         <v>4618</v>
       </c>
@@ -23606,7 +23604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="389" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:26">
       <c r="A389">
         <v>4601</v>
       </c>
@@ -23647,7 +23645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="390" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:26">
       <c r="A390">
         <v>4622</v>
       </c>
@@ -23688,7 +23686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="391" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:26">
       <c r="A391">
         <v>4616</v>
       </c>
@@ -23729,7 +23727,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="392" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:26">
       <c r="A392">
         <v>4601</v>
       </c>
@@ -23770,7 +23768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="393" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:26">
       <c r="A393">
         <v>4601</v>
       </c>
@@ -23817,7 +23815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="394" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:26">
       <c r="A394">
         <v>4621</v>
       </c>
@@ -23858,7 +23856,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="395" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:26">
       <c r="A395">
         <v>4610</v>
       </c>
@@ -23905,7 +23903,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="396" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:26">
       <c r="A396">
         <v>4605</v>
       </c>
@@ -23952,7 +23950,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="397" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:26">
       <c r="A397">
         <v>4618</v>
       </c>
@@ -23993,7 +23991,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="398" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:26">
       <c r="A398">
         <v>4611</v>
       </c>
@@ -24035,7 +24033,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="399" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:26">
       <c r="A399">
         <v>4601</v>
       </c>
@@ -24071,7 +24069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="400" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:26">
       <c r="A400">
         <v>4601</v>
       </c>
@@ -24118,7 +24116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="401" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:26">
       <c r="A401">
         <v>4602</v>
       </c>
@@ -24159,7 +24157,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="402" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:26">
       <c r="A402">
         <v>4607</v>
       </c>
@@ -24200,7 +24198,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="403" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:26">
       <c r="A403">
         <v>4612</v>
       </c>
@@ -24236,7 +24234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="404" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:26">
       <c r="A404">
         <v>4614</v>
       </c>
@@ -24278,7 +24276,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="405" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:26">
       <c r="A405">
         <v>4620</v>
       </c>
@@ -24319,7 +24317,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="406" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:26">
       <c r="A406">
         <v>4624</v>
       </c>
@@ -24361,7 +24359,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="407" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:26">
       <c r="A407">
         <v>4627</v>
       </c>
@@ -24397,7 +24395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="408" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:26">
       <c r="A408">
         <v>4627</v>
       </c>
@@ -24439,7 +24437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="409" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:26">
       <c r="A409">
         <v>4604</v>
       </c>
@@ -24480,7 +24478,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="410" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:26">
       <c r="A410">
         <v>4612</v>
       </c>
@@ -24527,7 +24525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="411" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:26">
       <c r="A411">
         <v>4624</v>
       </c>
@@ -24568,7 +24566,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="412" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:26">
       <c r="A412">
         <v>4618</v>
       </c>
@@ -24615,7 +24613,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="413" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:26">
       <c r="A413">
         <v>4618</v>
       </c>
@@ -24662,7 +24660,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="414" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:26">
       <c r="A414">
         <v>4603</v>
       </c>
@@ -24704,7 +24702,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="415" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:26">
       <c r="A415">
         <v>4601</v>
       </c>
@@ -24754,7 +24752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="416" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:26">
       <c r="A416">
         <v>4627</v>
       </c>
@@ -24796,7 +24794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="417" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:26">
       <c r="A417">
         <v>4612</v>
       </c>
@@ -24843,7 +24841,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="418" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:26">
       <c r="A418">
         <v>4624</v>
       </c>
@@ -24890,7 +24888,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="419" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:26">
       <c r="A419">
         <v>4627</v>
       </c>
@@ -24937,7 +24935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="420" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:26">
       <c r="A420">
         <v>4616</v>
       </c>
@@ -24984,7 +24982,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="421" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:26">
       <c r="A421">
         <v>4624</v>
       </c>
@@ -25031,7 +25029,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="422" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:26">
       <c r="A422">
         <v>4618</v>
       </c>
@@ -25067,7 +25065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="423" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:26">
       <c r="A423">
         <v>4625</v>
       </c>
@@ -25108,7 +25106,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="424" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:26">
       <c r="A424">
         <v>4611</v>
       </c>
@@ -25149,7 +25147,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="425" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:26">
       <c r="A425">
         <v>4618</v>
       </c>
@@ -25185,7 +25183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="426" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:26">
       <c r="A426">
         <v>4627</v>
       </c>
@@ -25232,7 +25230,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="427" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:26">
       <c r="A427">
         <v>4620</v>
       </c>
@@ -25279,7 +25277,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="428" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:26">
       <c r="A428">
         <v>4624</v>
       </c>
@@ -25320,7 +25318,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="429" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:26">
       <c r="A429">
         <v>4621</v>
       </c>
@@ -25367,7 +25365,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="430" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:26">
       <c r="A430">
         <v>4601</v>
       </c>
@@ -25416,7 +25414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="431" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:26">
       <c r="A431">
         <v>4612</v>
       </c>
@@ -25452,7 +25450,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="432" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:26">
       <c r="A432">
         <v>4612</v>
       </c>
@@ -25493,7 +25491,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="433" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:26">
       <c r="A433">
         <v>4624</v>
       </c>
@@ -25540,7 +25538,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="434" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:26">
       <c r="A434">
         <v>4619</v>
       </c>
@@ -25587,7 +25585,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="435" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:26">
       <c r="A435">
         <v>4605</v>
       </c>
@@ -25634,7 +25632,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="436" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:26">
       <c r="A436">
         <v>4604</v>
       </c>
@@ -25681,7 +25679,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="437" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:26">
       <c r="A437">
         <v>4627</v>
       </c>
@@ -25722,7 +25720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="438" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:26">
       <c r="A438">
         <v>4612</v>
       </c>
@@ -25764,7 +25762,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="439" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:26">
       <c r="A439">
         <v>4601</v>
       </c>
@@ -25805,7 +25803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="440" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:26">
       <c r="A440">
         <v>4603</v>
       </c>
@@ -25847,7 +25845,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="441" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:26">
       <c r="A441">
         <v>4601</v>
       </c>
@@ -25894,7 +25892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="442" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:26">
       <c r="A442">
         <v>4624</v>
       </c>
@@ -25941,7 +25939,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="443" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:26">
       <c r="A443">
         <v>4627</v>
       </c>
@@ -25982,7 +25980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="444" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:26">
       <c r="A444">
         <v>4601</v>
       </c>
@@ -26029,7 +26027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="445" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:26">
       <c r="A445">
         <v>4602</v>
       </c>
@@ -26070,7 +26068,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="446" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:26">
       <c r="A446">
         <v>4620</v>
       </c>
@@ -26117,7 +26115,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="447" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:26">
       <c r="A447">
         <v>4627</v>
       </c>
@@ -26153,7 +26151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="448" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:26">
       <c r="A448">
         <v>4603</v>
       </c>
@@ -26189,7 +26187,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="449" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:26">
       <c r="A449">
         <v>4604</v>
       </c>
@@ -26225,7 +26223,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="450" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:26">
       <c r="A450">
         <v>4602</v>
       </c>
@@ -26273,7 +26271,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="451" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:26">
       <c r="A451">
         <v>4611</v>
       </c>
@@ -26314,7 +26312,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="452" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:26">
       <c r="A452">
         <v>4619</v>
       </c>
@@ -26362,7 +26360,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="453" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:26">
       <c r="A453">
         <v>4627</v>
       </c>
@@ -26404,7 +26402,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="454" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:26">
       <c r="A454">
         <v>4627</v>
       </c>
@@ -26445,7 +26443,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="455" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:26">
       <c r="A455">
         <v>4627</v>
       </c>
@@ -26486,7 +26484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="456" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:26">
       <c r="A456">
         <v>4612</v>
       </c>
@@ -26527,7 +26525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="457" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:26">
       <c r="A457">
         <v>4602</v>
       </c>
@@ -26568,7 +26566,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="458" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:26">
       <c r="A458">
         <v>4602</v>
       </c>
@@ -26615,7 +26613,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="459" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:26">
       <c r="A459">
         <v>4621</v>
       </c>
@@ -26654,7 +26652,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="460" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:26">
       <c r="A460">
         <v>4616</v>
       </c>
@@ -26695,7 +26693,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="461" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:26">
       <c r="A461">
         <v>4617</v>
       </c>
@@ -26736,7 +26734,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="462" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:26">
       <c r="A462">
         <v>4603</v>
       </c>
@@ -26777,7 +26775,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="463" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:26">
       <c r="A463">
         <v>4601</v>
       </c>
@@ -26819,7 +26817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="464" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:26">
       <c r="A464">
         <v>4601</v>
       </c>
@@ -26866,7 +26864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="465" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:26">
       <c r="A465">
         <v>4625</v>
       </c>
@@ -26902,7 +26900,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="466" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:26">
       <c r="A466">
         <v>4603</v>
       </c>
@@ -26938,7 +26936,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="467" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:26">
       <c r="A467">
         <v>4627</v>
       </c>
@@ -26979,7 +26977,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="468" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:26">
       <c r="A468">
         <v>4605</v>
       </c>
@@ -27015,7 +27013,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="469" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:26">
       <c r="A469">
         <v>4614</v>
       </c>
@@ -27062,7 +27060,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="470" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:26">
       <c r="A470">
         <v>4616</v>
       </c>
@@ -27104,7 +27102,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="471" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:26">
       <c r="A471">
         <v>4601</v>
       </c>
@@ -27145,7 +27143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="472" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:26">
       <c r="A472">
         <v>4601</v>
       </c>
@@ -27181,7 +27179,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="473" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:26">
       <c r="A473">
         <v>4612</v>
       </c>
@@ -27217,7 +27215,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="474" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:26">
       <c r="A474">
         <v>4626</v>
       </c>
@@ -27264,7 +27262,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="475" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:26">
       <c r="A475">
         <v>4603</v>
       </c>
@@ -27311,7 +27309,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="476" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:26">
       <c r="A476">
         <v>4627</v>
       </c>
@@ -27352,7 +27350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="477" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:26">
       <c r="A477">
         <v>4628</v>
       </c>
@@ -27394,7 +27392,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="478" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:26">
       <c r="A478">
         <v>4601</v>
       </c>
@@ -27441,7 +27439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="479" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:26">
       <c r="A479">
         <v>4601</v>
       </c>
@@ -27488,7 +27486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="480" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:26">
       <c r="A480">
         <v>4620</v>
       </c>
@@ -27535,7 +27533,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="481" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:26">
       <c r="A481">
         <v>4624</v>
       </c>
@@ -27582,7 +27580,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="482" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:26">
       <c r="A482">
         <v>4624</v>
       </c>
@@ -27629,7 +27627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="483" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:26">
       <c r="A483">
         <v>4624</v>
       </c>
@@ -27670,7 +27668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="484" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:26">
       <c r="A484">
         <v>4601</v>
       </c>
@@ -27711,7 +27709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="485" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:26">
       <c r="A485">
         <v>4601</v>
       </c>
@@ -27752,7 +27750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="486" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:26">
       <c r="A486">
         <v>4602</v>
       </c>
@@ -27788,7 +27786,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="487" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:26">
       <c r="A487">
         <v>4605</v>
       </c>
@@ -27830,7 +27828,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="488" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:26">
       <c r="A488">
         <v>4601</v>
       </c>
@@ -27877,7 +27875,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="489" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:26">
       <c r="A489">
         <v>4621</v>
       </c>
@@ -27918,7 +27916,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="490" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:26">
       <c r="A490">
         <v>4621</v>
       </c>
@@ -27965,7 +27963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="491" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:26">
       <c r="A491">
         <v>4601</v>
       </c>
@@ -28009,7 +28007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="492" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:26">
       <c r="A492">
         <v>4620</v>
       </c>
@@ -28056,7 +28054,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="493" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:26">
       <c r="A493">
         <v>4601</v>
       </c>
@@ -28103,7 +28101,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="494" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:26">
       <c r="A494">
         <v>4603</v>
       </c>
@@ -28150,7 +28148,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="495" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:26">
       <c r="A495">
         <v>4604</v>
       </c>
@@ -28197,7 +28195,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="496" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:26">
       <c r="A496">
         <v>4618</v>
       </c>
@@ -28238,7 +28236,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="497" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:26">
       <c r="A497">
         <v>4601</v>
       </c>
@@ -28279,7 +28277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="498" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:26">
       <c r="A498">
         <v>4618</v>
       </c>
@@ -28326,7 +28324,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="499" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:26">
       <c r="A499">
         <v>4624</v>
       </c>
@@ -28370,7 +28368,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="500" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:26">
       <c r="A500">
         <v>4624</v>
       </c>
@@ -28428,24 +28426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>